<commit_message>
Adicionando formulas MAIOR, MENOR combinado com SE
</commit_message>
<xml_diff>
--- a/SOMASES/SOMASES.xlsx
+++ b/SOMASES/SOMASES.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OneDrive for Business\Estudo\python\excel_to_pandas\SOMASES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C1A6891-D5E1-49BD-A23F-C36433C71CF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66128194-52C6-47EC-8D62-85BABBC73848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PIB" sheetId="1" r:id="rId1"/>
@@ -488,9 +488,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2941,7 +2939,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3213,7 +3211,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>